<commit_message>
Did a TestRun not done yet
</commit_message>
<xml_diff>
--- a/DTT Assessment/DTT-Assessment-Hour-Log-1_updated_bonus.xlsx
+++ b/DTT Assessment/DTT-Assessment-Hour-Log-1_updated_bonus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d9630c1c7287dc4/Documenten/Bit acedemy/DTT/DTT-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d9630c1c7287dc4/Documenten/Bit acedemy/Zero/DTT/DTT Assessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B59C7380-0F5F-49F6-8E4F-F17B6764DE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{B59C7380-0F5F-49F6-8E4F-F17B6764DE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{387BE743-322E-4CC2-BE49-39066996E0E3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1727,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1759,7 +1758,7 @@
       <c r="E2" s="23"/>
       <c r="F2" s="24"/>
     </row>
-    <row r="3" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1777,7 +1776,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1793,7 +1792,7 @@
       <c r="E4" s="20"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1809,7 +1808,7 @@
       <c r="E5" s="20"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
@@ -1825,7 +1824,7 @@
       <c r="E6" s="20"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1841,12 +1840,12 @@
       <c r="E7" s="20"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="17">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="18">
         <v>44978</v>
@@ -1857,7 +1856,7 @@
       <c r="E8" s="20"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1873,7 +1872,7 @@
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
@@ -1881,7 +1880,7 @@
       <c r="E10" s="20"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
@@ -1889,7 +1888,7 @@
       <c r="E11" s="20"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -1897,7 +1896,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="17"/>
       <c r="C13" s="18"/>
@@ -1905,7 +1904,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -1913,7 +1912,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -1921,7 +1920,7 @@
       <c r="E15" s="20"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -1929,7 +1928,7 @@
       <c r="E16" s="20"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -1937,7 +1936,7 @@
       <c r="E17" s="20"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
@@ -1945,7 +1944,7 @@
       <c r="E18" s="20"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="17"/>
       <c r="C19" s="18"/>
@@ -1953,7 +1952,7 @@
       <c r="E19" s="20"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -1961,7 +1960,7 @@
       <c r="E20" s="20"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
@@ -1969,7 +1968,7 @@
       <c r="E21" s="20"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="17"/>
       <c r="C22" s="18"/>
@@ -1977,7 +1976,7 @@
       <c r="E22" s="20"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
@@ -1985,7 +1984,7 @@
       <c r="E23" s="20"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
@@ -1993,7 +1992,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="17"/>
       <c r="C25" s="18"/>
@@ -2001,7 +2000,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
@@ -2009,7 +2008,7 @@
       <c r="E26" s="20"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="17"/>
       <c r="C27" s="18"/>
@@ -2017,7 +2016,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
@@ -2025,7 +2024,7 @@
       <c r="E28" s="20"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -2033,13 +2032,13 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>